<commit_message>
shortwave mls H2O. download links for summary tables
</commit_message>
<xml_diff>
--- a/shortwave/shortwave_mls_H2O_by_clirad_bands.xlsx
+++ b/shortwave/shortwave_mls_H2O_by_clirad_bands.xlsx
@@ -1558,10 +1558,10 @@
         <v>-1.66207709288212e-13</v>
       </c>
       <c r="E13">
-        <v>-2.09240668258559e-06</v>
+        <v>-2.09240668169741e-06</v>
       </c>
       <c r="F13">
-        <v>-2.09240684956313e-06</v>
+        <v>-2.09240684867495e-06</v>
       </c>
       <c r="G13">
         <v>0.005518143</v>
@@ -1579,10 +1579,10 @@
         <v>-7.12540115773546e-14</v>
       </c>
       <c r="E14">
-        <v>-2.19702701631519e-05</v>
+        <v>-2.19702701622637e-05</v>
       </c>
       <c r="F14">
-        <v>-2.19702702350943e-05</v>
+        <v>-2.19702702342062e-05</v>
       </c>
       <c r="G14">
         <v>1.61076e-07</v>
@@ -1600,10 +1600,10 @@
         <v>-0</v>
       </c>
       <c r="E15">
-        <v>-3.55709135959614e-05</v>
+        <v>-3.55709135950733e-05</v>
       </c>
       <c r="F15">
-        <v>-3.55709135959614e-05</v>
+        <v>-3.55709135950733e-05</v>
       </c>
       <c r="G15">
         <v>1.610757e-07</v>
@@ -1665,10 +1665,10 @@
         <v>-0</v>
       </c>
       <c r="E18">
-        <v>7.9104775230864</v>
+        <v>7.91047752308641</v>
       </c>
       <c r="F18">
-        <v>7.9104775230864</v>
+        <v>7.91047752308641</v>
       </c>
       <c r="G18">
         <v>2.88006e-08</v>
@@ -2878,10 +2878,10 @@
         <v>-0.000147480834985101</v>
       </c>
       <c r="E13">
-        <v>-0.000199835547903149</v>
+        <v>-0.000199835547931571</v>
       </c>
       <c r="F13">
-        <v>-0.000347316382885765</v>
+        <v>-0.000347316382914187</v>
       </c>
       <c r="G13">
         <v>0.47568947861</v>
@@ -2899,10 +2899,10 @@
         <v>-5.91856718329486e-05</v>
       </c>
       <c r="E14">
-        <v>0.0429418961012402</v>
+        <v>0.0429418961012118</v>
       </c>
       <c r="F14">
-        <v>0.0428827104294385</v>
+        <v>0.0428827104294101</v>
       </c>
       <c r="G14">
         <v>0.00541452166896558</v>
@@ -2943,10 +2943,10 @@
         <v>-0.000147480834985101</v>
       </c>
       <c r="E16">
-        <v>-0.000199785547891906</v>
+        <v>-0.000199785547920328</v>
       </c>
       <c r="F16">
-        <v>-0.000347266382874523</v>
+        <v>-0.000347266382902944</v>
       </c>
       <c r="G16">
         <v>0.47659577308</v>
@@ -2964,10 +2964,10 @@
         <v>-5.91856718329486e-05</v>
       </c>
       <c r="E17">
-        <v>0.102964776101572</v>
+        <v>0.102964776101544</v>
       </c>
       <c r="F17">
-        <v>0.102905590429771</v>
+        <v>0.102905590429742</v>
       </c>
       <c r="G17">
         <v>-0.00137736944372172</v>

</xml_diff>